<commit_message>
Worked on the effects doc. + Finished cleaning the Druid skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/7-Druide/Documentation/DruidSkills.xlsx
+++ b/GameDesign/Class/_Done/7-Druide/Documentation/DruidSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-FountainOfImmortality" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>Additional Info</t>
   </si>
@@ -137,33 +137,12 @@
     <t>[[Range: 0-6 ]]</t>
   </si>
   <si>
-    <t>On ennemy: [[Increase cooldown of all skills by 1 ]]</t>
-  </si>
-  <si>
-    <t>On self OR allie: [[Reduce cooldown of all skills by 1 ]]</t>
-  </si>
-  <si>
-    <t>Increase the cooldown of an ennemie skills.                                        OR                                                                                                Reduce the cooldown of the caster or an allie skills.</t>
-  </si>
-  <si>
     <t>Advanced Medicine</t>
   </si>
   <si>
     <t>[[AP: 6 ]]</t>
   </si>
   <si>
-    <t>On caster or allie: (caster: [[Reduce max HP by 5%]] (00 turns))</t>
-  </si>
-  <si>
-    <t>Effect name: ''Void''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Slowness''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Exhausted''.</t>
-  </si>
-  <si>
     <t>[[Number of casts per turn: 1 ]]</t>
   </si>
   <si>
@@ -179,27 +158,9 @@
     <t>Inflicts Water-type damage on ennemies                                             OR                                                                                                     Heal Water-type on caster and allies.</t>
   </si>
   <si>
-    <t>On caster or allie: [[Reduce MP by 1]]                         (00 turns)</t>
-  </si>
-  <si>
-    <t>On caster or allie: [[Reduce AP by 1]]                          (00 turns)</t>
-  </si>
-  <si>
-    <t>On ennemy: (caster: [[Reduce max HP by 10%]]        (00 turns))</t>
-  </si>
-  <si>
-    <t>On ennemy: [[Reduce AP by 1]]                                   (2 turns)</t>
-  </si>
-  <si>
-    <t>On ennemy: [[Reduce MP by 1]]                                  (2 turns)</t>
-  </si>
-  <si>
     <t>Animal Sacrifice</t>
   </si>
   <si>
-    <t>On allie summon: [[Kill the target]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Target adjacent cells ]]</t>
   </si>
   <si>
@@ -209,15 +170,6 @@
     <t xml:space="preserve">Inflicts Fire-type damage on ennemies and heal Light-type the entity around.                                                                                                OR                                                                                                        Kill an allie summon and heal Light-type the entity around.                                                                                                                            </t>
   </si>
   <si>
-    <t>On ennemy: [[Damage: 35-40 fire]]</t>
-  </si>
-  <si>
-    <t>On ennemy: (entity in the area: [[Heal: 10-15 light]])</t>
-  </si>
-  <si>
-    <t>On allie summon: (entity in the area: [[Heal: 50-75 light]])</t>
-  </si>
-  <si>
     <t>[[Number of cast per turn per target: 2 ]]</t>
   </si>
   <si>
@@ -227,12 +179,6 @@
     <t>On ennemy: [[Damage:  35-40 water ]]</t>
   </si>
   <si>
-    <t>On caster or allie: [[Heal: 200-250 light ]]</t>
-  </si>
-  <si>
-    <t>On ennemy: [[Damage: 100-125 light ]]</t>
-  </si>
-  <si>
     <t>Imbolc</t>
   </si>
   <si>
@@ -248,24 +194,6 @@
     <t>[[Area of effect: - Square of 1 cell radius around the target ]]</t>
   </si>
   <si>
-    <t>Self and allies: [[Heal: 15% of their max HP]]</t>
-  </si>
-  <si>
-    <t>Effect name: ''Imbolc''.</t>
-  </si>
-  <si>
-    <t>Entities: [[Reduce all buff by 3 turns]]</t>
-  </si>
-  <si>
-    <t>Effect name: ''Beltaine''.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Hard Skin''.</t>
-  </si>
-  <si>
-    <t>Entities: [[Reduce taken damages by 25%]] (2 turns)</t>
-  </si>
-  <si>
     <t>Beltane</t>
   </si>
   <si>
@@ -275,24 +203,9 @@
     <t>[[Area of effect: - All the map ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Lugnasa''.</t>
-  </si>
-  <si>
-    <t>On entities: [[Heal 50% of their max HP]]</t>
-  </si>
-  <si>
-    <t>Heal all the entities in the map.                                                       The effect is triggered the next turn around the caster.</t>
-  </si>
-  <si>
-    <t>Reduce damage taken by entities.                                                       The effect is triggered the next turn around the caster.</t>
-  </si>
-  <si>
     <t>Reduce all the buff of the entities and heal the caster and his allies. The effect is triggered the next turn around the caster.</t>
   </si>
   <si>
-    <t>Inflicts Light-type damage on ennemies                                             OR                                                                                                     Heal Light-type on caster and allies.                                                                                                                            Also reduce the target AP and MP whit a duration depending of the target.                                                                                                The caster life expectancy is reduced.</t>
-  </si>
-  <si>
     <t>Summons a ''Fountain Of Immortality'' [[75% summoner HP, 0 AP, 0 MP, -50% ground resistence, -25% fire resistence, 50% water resistence, 25% wind resistence, 100% light resistence, -100% dark resistence]]</t>
   </si>
   <si>
@@ -420,6 +333,252 @@
   </si>
   <si>
     <t>[[Reduce all buff by 1 turn ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Laziness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +1 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Slowness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+1 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Void]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Targeting an ennemy: </t>
+  </si>
+  <si>
+    <t>Targeting the caster or an ally:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Heal: 200-250 light ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Laziness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +1 level (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Slowness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+1 level (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Caster: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Void]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +5 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 100-125 fire ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage on ennemies                                               OR                                                                                                     Heal Light-type on caster and allies.                                                                                                                            Also reduce the target AP and MP whit a duration depending of the target.                                                                                                The caster life expectancy is reduced.</t>
+  </si>
+  <si>
+    <t>Targeting caster summon or ally summon:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    In the area of effect: [[Heal: 50-75 light]]</t>
+  </si>
+  <si>
+    <t>Targeting enemy:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    In the area of effect: [[Heal: 10-15 light]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Targeted cell: [[Damage: 35-40 fire]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Targeted cell: [[K/O]]</t>
+  </si>
+  <si>
+    <t>Increase the cooldown of an enemy skills already in a cooldown process.                                                                                                    OR                                                                                                Reduce the cooldown of the caster or an ally skills.</t>
+  </si>
+  <si>
+    <t>On ennemy: [[Increase skills cooldown by 1 ]]</t>
+  </si>
+  <si>
+    <t>On self OR ally: [[Reduce skills cooldown by 1 ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Imbolc]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Beltane]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Heal all the entities in the map.                                                       The effect is triggered the next turn.</t>
+  </si>
+  <si>
+    <t>Reduce damage taken.                                                                            The effect is triggered the next turn around the caster.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Lugnasa]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -491,7 +650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -541,71 +700,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -625,11 +719,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -655,13 +758,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,49 +1198,49 @@
     <row r="19" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="17" t="s">
-        <v>87</v>
+      <c r="C20" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="19" t="s">
-        <v>88</v>
+      <c r="C21" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="18" t="s">
-        <v>90</v>
+      <c r="C22" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="18" t="s">
-        <v>91</v>
+      <c r="C23" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="18" t="s">
-        <v>92</v>
+      <c r="C24" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="19" t="s">
-        <v>89</v>
+      <c r="C25" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1188,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G7"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1308,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1221,7 +1320,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1247,7 +1346,7 @@
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1259,7 +1358,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1283,7 +1382,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1295,7 +1394,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1324,9 +1423,7 @@
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1465,7 +1562,7 @@
     <row r="19" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1527,7 +1624,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1737,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1687,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1817,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1784,7 +1881,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1808,14 +1905,14 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="9" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="9" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1863,7 +1960,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1980,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1895,7 +1992,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1907,14 +2004,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1926,7 +2023,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1940,7 +2037,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1952,7 +2049,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1968,7 +2065,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1976,101 +2073,99 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="14" t="s">
-        <v>51</v>
+      <c r="C19" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>52</v>
+      <c r="C20" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="11" t="s">
-        <v>50</v>
+      <c r="C21" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="13" t="s">
-        <v>64</v>
+      <c r="C22" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="14" t="s">
-        <v>49</v>
+      <c r="C23" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="14" t="s">
-        <v>48</v>
+      <c r="C24" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="12" t="s">
-        <v>39</v>
+      <c r="C25" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
+    <row r="29" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B31" s="1"/>
-      <c r="C31" s="7" t="s">
-        <v>42</v>
+      <c r="C31" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B33" s="1"/>
-      <c r="C33" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="C33" s="7"/>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -2086,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,7 +2204,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2121,7 +2216,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2178,7 +2273,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2197,75 +2292,89 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>54</v>
+      <c r="C19" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="16" t="s">
-        <v>60</v>
+      <c r="C20" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="15" t="s">
-        <v>58</v>
+      <c r="C21" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
-        <v>59</v>
+      <c r="C22" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
+    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B30" s="1"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2307,10 +2416,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2391,14 +2500,14 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2443,7 +2552,161 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D24"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -2466,7 +2729,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2478,7 +2741,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2490,7 +2753,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2504,7 +2767,7 @@
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2516,7 +2779,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2528,7 +2791,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2540,7 +2803,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2552,170 +2815,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2744,22 +2844,13 @@
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>